<commit_message>
Can now generate TreasureChestsls!
</commit_message>
<xml_diff>
--- a/tests/data/test_google_drive_data/settings.xlsx
+++ b/tests/data/test_google_drive_data/settings.xlsx
@@ -11,12 +11,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
   <si>
+    <t>Total Reward</t>
+  </si>
+  <si>
+    <t>Total Savings</t>
+  </si>
+  <si>
+    <t>Total Tokens</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
     <t>steven</t>
+  </si>
+  <si>
+    <t>connie</t>
   </si>
 </sst>
 </file>
@@ -73,15 +88,61 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="14.0"/>
+    <col customWidth="1" min="3" max="3" width="13.43"/>
+    <col customWidth="1" min="4" max="4" width="13.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked variable names, added a print function.
</commit_message>
<xml_diff>
--- a/tests/data/test_google_drive_data/settings.xlsx
+++ b/tests/data/test_google_drive_data/settings.xlsx
@@ -13,10 +13,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Username</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Total Reward</t>
+    <t>Total Loot</t>
   </si>
   <si>
     <t>Total Savings</t>

</xml_diff>

<commit_message>
Changed how we decide how much gold is distributed per token. Now we base the amount off of a setting, Gold per Value.
</commit_message>
<xml_diff>
--- a/tests/data/test_google_drive_data/settings.xlsx
+++ b/tests/data/test_google_drive_data/settings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -25,10 +25,13 @@
     <t>Total Tokens</t>
   </si>
   <si>
-    <t>Tokens Per Hour</t>
+    <t>Tokens per Hour</t>
   </si>
   <si>
     <t>Total Time</t>
+  </si>
+  <si>
+    <t>Gold per Value</t>
   </si>
   <si>
     <t>steven</t>
@@ -74,7 +77,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -125,10 +128,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>10.0</v>
@@ -145,10 +151,13 @@
       <c r="F2" s="1">
         <v>720.0</v>
       </c>
+      <c r="G2" s="1">
+        <v>1000.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>5.0</v>
@@ -165,6 +174,9 @@
       <c r="F3" s="1">
         <v>720.0</v>
       </c>
+      <c r="G3" s="1">
+        <v>1000.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>